<commit_message>
come out the reporting result
</commit_message>
<xml_diff>
--- a/Sray/Analysis/AU/AU_Descriptive Statistics.xlsx
+++ b/Sray/Analysis/AU/AU_Descriptive Statistics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="main" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="sec_no_count" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="kurtosis" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="main" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sec_no_count" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="kurtosis" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +17,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <name val="Calibri"/>
@@ -100,11 +102,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -475,7 +478,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y12"/>
+  <dimension ref="A1:AC14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -556,50 +559,70 @@
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
+          <t>ret</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
           <t>historical_market_cap</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>trail_12m_sales_per_sh</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>is_eps</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>fcf</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>pe</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>return_com_eqy</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>roa</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>VOLATILITY_180D</t>
-        </is>
-      </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>volatility_360d</t>
+          <t>roa_sec_mean</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>roa_sec_sd</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>roa_z</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>vol_180d</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>vol_360d</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>beta</t>
         </is>
@@ -612,76 +635,88 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>18704</v>
+        <v>2338</v>
       </c>
       <c r="C2" t="n">
-        <v>18704</v>
+        <v>2338</v>
       </c>
       <c r="D2" t="n">
-        <v>18704</v>
+        <v>2338</v>
       </c>
       <c r="E2" t="n">
-        <v>18704</v>
+        <v>2338</v>
       </c>
       <c r="F2" t="n">
-        <v>18704</v>
+        <v>2338</v>
       </c>
       <c r="G2" t="n">
-        <v>14840</v>
+        <v>1847</v>
       </c>
       <c r="H2" t="n">
-        <v>14840</v>
+        <v>1847</v>
       </c>
       <c r="I2" t="n">
-        <v>14840</v>
+        <v>1847</v>
       </c>
       <c r="J2" t="n">
-        <v>14840</v>
+        <v>1847</v>
       </c>
       <c r="K2" t="n">
-        <v>14840</v>
+        <v>1847</v>
       </c>
       <c r="L2" t="n">
-        <v>14840</v>
+        <v>1847</v>
       </c>
       <c r="M2" t="n">
-        <v>14840</v>
+        <v>1847</v>
       </c>
       <c r="N2" t="n">
-        <v>14840</v>
+        <v>1847</v>
       </c>
       <c r="O2" t="n">
-        <v>18018</v>
+        <v>2267</v>
       </c>
       <c r="P2" t="n">
-        <v>17969</v>
+        <v>1934</v>
       </c>
       <c r="Q2" t="n">
-        <v>17885</v>
+        <v>2260</v>
       </c>
       <c r="R2" t="n">
-        <v>18109</v>
+        <v>2252</v>
       </c>
       <c r="S2" t="n">
-        <v>18144</v>
+        <v>2276</v>
       </c>
       <c r="T2" t="n">
-        <v>14658</v>
+        <v>2284</v>
       </c>
       <c r="U2" t="n">
-        <v>17745</v>
+        <v>1867</v>
       </c>
       <c r="V2" t="n">
-        <v>17927</v>
+        <v>2239</v>
       </c>
       <c r="W2" t="n">
-        <v>17836</v>
+        <v>2257</v>
       </c>
       <c r="X2" t="n">
-        <v>17689</v>
+        <v>2338</v>
       </c>
       <c r="Y2" t="n">
-        <v>17976</v>
+        <v>2331</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>2250</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>2245</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>2227</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>2262</v>
       </c>
     </row>
     <row r="3">
@@ -716,10 +751,8 @@
           <t>BPT AU Equity</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2017-12</t>
-        </is>
+      <c r="F4" s="2" t="n">
+        <v>43100</v>
       </c>
     </row>
     <row r="5">
@@ -729,502 +762,606 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="C5" t="n">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
-        <v>4676</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>mean</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>5.077844311377246</v>
-      </c>
-      <c r="E6" t="n">
-        <v>2019.625</v>
-      </c>
-      <c r="G6" t="n">
-        <v>34.31315040723333</v>
-      </c>
-      <c r="H6" t="n">
-        <v>71.10073857397403</v>
-      </c>
-      <c r="I6" t="n">
-        <v>18.92584590594161</v>
-      </c>
-      <c r="J6" t="n">
-        <v>12.776707727448</v>
-      </c>
-      <c r="K6" t="n">
-        <v>416.0941649480384</v>
-      </c>
-      <c r="L6" t="n">
-        <v>984.3335416916592</v>
-      </c>
-      <c r="M6" t="n">
-        <v>1409.931877941888</v>
-      </c>
-      <c r="N6" t="n">
-        <v>55720.24542194306</v>
-      </c>
-      <c r="O6" t="n">
-        <v>8.863444794094795</v>
-      </c>
-      <c r="P6" t="n">
-        <v>3744.648882430853</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>3.930384187866927</v>
-      </c>
-      <c r="R6" t="n">
-        <v>0.196132083494395</v>
-      </c>
-      <c r="S6" t="n">
-        <v>100.2549524691358</v>
-      </c>
-      <c r="T6" t="n">
-        <v>60.95623767908309</v>
-      </c>
-      <c r="U6" t="n">
-        <v>2.258265759368836</v>
-      </c>
-      <c r="V6" t="n">
-        <v>-1.252337641546271</v>
-      </c>
-      <c r="W6" t="n">
-        <v>48.93987323390895</v>
-      </c>
-      <c r="X6" t="n">
-        <v>50.14629362880886</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>1.048477842679128</v>
+          <t>first</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>43100</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>std</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>3.077903291964363</v>
-      </c>
-      <c r="E7" t="n">
-        <v>2.117690904661095</v>
-      </c>
-      <c r="G7" t="n">
-        <v>11.61100419275182</v>
-      </c>
-      <c r="H7" t="n">
-        <v>11.45154716562464</v>
-      </c>
-      <c r="I7" t="n">
-        <v>12.54694598323816</v>
-      </c>
-      <c r="J7" t="n">
-        <v>17.22359298093507</v>
-      </c>
-      <c r="K7" t="n">
-        <v>740.1854770476324</v>
-      </c>
-      <c r="L7" t="n">
-        <v>1389.073715130661</v>
-      </c>
-      <c r="M7" t="n">
-        <v>1052.202377887494</v>
-      </c>
-      <c r="N7" t="n">
-        <v>63046.01961833036</v>
-      </c>
-      <c r="O7" t="n">
-        <v>23.46239909386085</v>
-      </c>
-      <c r="P7" t="n">
-        <v>10031.16701091441</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>8.413662912072224</v>
-      </c>
-      <c r="R7" t="n">
-        <v>1.036766826515721</v>
-      </c>
-      <c r="S7" t="n">
-        <v>1499.25995592581</v>
-      </c>
-      <c r="T7" t="n">
-        <v>255.5217149532694</v>
-      </c>
-      <c r="U7" t="n">
-        <v>154.7289088862799</v>
-      </c>
-      <c r="V7" t="n">
-        <v>25.82975969790617</v>
-      </c>
-      <c r="W7" t="n">
-        <v>30.12405042933933</v>
-      </c>
-      <c r="X7" t="n">
-        <v>29.22511996741768</v>
-      </c>
-      <c r="Y7" t="n">
-        <v>1.202723569784605</v>
+          <t>last</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>44957</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>min</t>
+          <t>mean</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>5.077844311377246</v>
       </c>
       <c r="E8" t="n">
-        <v>2017</v>
+        <v>2020</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>34.66641053032991</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>71.23302684013561</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>19.30656206830489</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>13.32424265857832</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>434.5488044046775</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>1026.658732672436</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
+        <v>1440.821046048497</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>57371.55100039794</v>
       </c>
       <c r="O8" t="n">
-        <v>0.002</v>
+        <v>8.984893250992501</v>
       </c>
       <c r="P8" t="n">
-        <v>1.086</v>
+        <v>0.120638951479052</v>
       </c>
       <c r="Q8" t="n">
-        <v>-0.4421</v>
+        <v>3807.935974469026</v>
       </c>
       <c r="R8" t="n">
-        <v>-3.92</v>
+        <v>3.966047690941386</v>
       </c>
       <c r="S8" t="n">
-        <v>-31240</v>
+        <v>0.19632460456942</v>
       </c>
       <c r="T8" t="n">
-        <v>0.0422</v>
+        <v>110.2814411120841</v>
       </c>
       <c r="U8" t="n">
-        <v>-1152.539</v>
+        <v>64.51987198714515</v>
       </c>
       <c r="V8" t="n">
-        <v>-251.5547</v>
+        <v>2.581755783832068</v>
       </c>
       <c r="W8" t="n">
-        <v>10.265</v>
+        <v>-1.108594683207798</v>
       </c>
       <c r="X8" t="n">
-        <v>10.538</v>
+        <v>-1.077204776322566</v>
       </c>
       <c r="Y8" t="n">
-        <v>-13.1442</v>
+        <v>21.6135268750835</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>1.1842378929335e-17</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>49.82201202672606</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>50.83442478670857</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>1.088424977895667</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>25%</t>
+          <t>std</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>3.078479439448217</v>
       </c>
       <c r="E9" t="n">
-        <v>2017.75</v>
+        <v>2.000427853251231</v>
       </c>
       <c r="G9" t="n">
-        <v>26.63967418670654</v>
+        <v>11.72760405250256</v>
       </c>
       <c r="H9" t="n">
-        <v>63.5761604309082</v>
+        <v>11.50367574821878</v>
       </c>
       <c r="I9" t="n">
-        <v>10.54262399673462</v>
+        <v>12.6658289986203</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>17.45951863474469</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>753.3599236010529</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>1409.495183691039</v>
       </c>
       <c r="M9" t="n">
-        <v>695.0869643130809</v>
+        <v>1064.00231838497</v>
       </c>
       <c r="N9" t="n">
-        <v>18905.45091790054</v>
+        <v>64178.44459521989</v>
       </c>
       <c r="O9" t="n">
-        <v>0.77</v>
+        <v>24.01001406528078</v>
       </c>
       <c r="P9" t="n">
-        <v>249.8972</v>
+        <v>0.9414744174950912</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.2374</v>
+        <v>10143.5379122734</v>
       </c>
       <c r="R9" t="n">
-        <v>-0.0069</v>
+        <v>8.52459914251658</v>
       </c>
       <c r="S9" t="n">
-        <v>-8.82865</v>
+        <v>1.017267584956456</v>
       </c>
       <c r="T9" t="n">
-        <v>10.4679</v>
+        <v>1548.03533103011</v>
       </c>
       <c r="U9" t="n">
-        <v>-7.6429</v>
+        <v>269.7182591850705</v>
       </c>
       <c r="V9" t="n">
-        <v>-4.7019</v>
+        <v>163.9337889919617</v>
       </c>
       <c r="W9" t="n">
-        <v>28.842</v>
+        <v>25.24287517450755</v>
       </c>
       <c r="X9" t="n">
-        <v>29.893</v>
+        <v>6.89847912434971</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.502775</v>
+        <v>11.7358757497773</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>0.9829583934233549</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>30.32218723906779</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>29.32624895085411</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>1.189226100974378</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>50%</t>
+          <t>min</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>2019.5</v>
+        <v>2017</v>
       </c>
       <c r="G10" t="n">
-        <v>30.97776889801025</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>75.46658325195312</v>
+        <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>14.72188568115234</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>2.506795883178711</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>36.5765355100699</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>185.5417149268287</v>
+        <v>0</v>
       </c>
       <c r="M10" t="n">
-        <v>1052.431043488873</v>
+        <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>29726.95603649999</v>
+        <v>0</v>
       </c>
       <c r="O10" t="n">
-        <v>2.6904</v>
+        <v>0.002</v>
       </c>
       <c r="P10" t="n">
-        <v>762.203</v>
+        <v>-0.9892945054028119</v>
       </c>
       <c r="Q10" t="n">
-        <v>1.0401</v>
+        <v>1.086</v>
       </c>
       <c r="R10" t="n">
-        <v>0.0483</v>
+        <v>-0.4421</v>
       </c>
       <c r="S10" t="n">
-        <v>4.402</v>
+        <v>-3.92</v>
       </c>
       <c r="T10" t="n">
-        <v>18.19365</v>
+        <v>-31240</v>
       </c>
       <c r="U10" t="n">
-        <v>7.6733</v>
+        <v>0.0422</v>
       </c>
       <c r="V10" t="n">
-        <v>3.5509</v>
+        <v>-1152.539</v>
       </c>
       <c r="W10" t="n">
-        <v>40.7775</v>
+        <v>-251.4689</v>
       </c>
       <c r="X10" t="n">
-        <v>42.454</v>
+        <v>-16.64057</v>
       </c>
       <c r="Y10" t="n">
-        <v>1.01875</v>
+        <v>2.706187555869</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>-5.796305928626865</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>10.265</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>10.538</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>-13.1442</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>75%</t>
+          <t>25%</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E11" t="n">
-        <v>2021.25</v>
+        <v>2018</v>
       </c>
       <c r="G11" t="n">
-        <v>40.1443510055542</v>
+        <v>26.97917747497559</v>
       </c>
       <c r="H11" t="n">
-        <v>78.59722900390625</v>
+        <v>63.5761604309082</v>
       </c>
       <c r="I11" t="n">
-        <v>25.22672367095947</v>
+        <v>10.58041095733643</v>
       </c>
       <c r="J11" t="n">
-        <v>20.9000301361084</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>502.3268842215622</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>1542.780310332222</v>
+        <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>1851.174355011681</v>
+        <v>706.6071246546161</v>
       </c>
       <c r="N11" t="n">
-        <v>64695.40886770176</v>
+        <v>19637.49624852485</v>
       </c>
       <c r="O11" t="n">
-        <v>7.1</v>
+        <v>0.7622</v>
       </c>
       <c r="P11" t="n">
-        <v>2623.344</v>
+        <v>-0.1980439148618991</v>
       </c>
       <c r="Q11" t="n">
-        <v>3.5203</v>
+        <v>259.3999</v>
       </c>
       <c r="R11" t="n">
-        <v>0.1717</v>
+        <v>0.23865</v>
       </c>
       <c r="S11" t="n">
-        <v>48.13175</v>
+        <v>-0.0069</v>
       </c>
       <c r="T11" t="n">
-        <v>33.2325</v>
+        <v>-9.11875</v>
       </c>
       <c r="U11" t="n">
-        <v>16.7569</v>
+        <v>10.4317</v>
       </c>
       <c r="V11" t="n">
-        <v>8.629899999999999</v>
+        <v>-7.9456</v>
       </c>
       <c r="W11" t="n">
-        <v>61.5975</v>
+        <v>-4.7657</v>
       </c>
       <c r="X11" t="n">
-        <v>62.917</v>
+        <v>-8.171819178082192</v>
       </c>
       <c r="Y11" t="n">
-        <v>1.568625</v>
+        <v>10.76062400204691</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>-0.3725976106666954</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>29.729</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>30.77</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>0.55575</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
+          <t>50%</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>4</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2020</v>
+      </c>
+      <c r="G12" t="n">
+        <v>31.22422218322754</v>
+      </c>
+      <c r="H12" t="n">
+        <v>75.52679443359375</v>
+      </c>
+      <c r="I12" t="n">
+        <v>15.08464336395264</v>
+      </c>
+      <c r="J12" t="n">
+        <v>2.92962908744812</v>
+      </c>
+      <c r="K12" t="n">
+        <v>47.65179660420357</v>
+      </c>
+      <c r="L12" t="n">
+        <v>222.6364775633983</v>
+      </c>
+      <c r="M12" t="n">
+        <v>1078.908950409721</v>
+      </c>
+      <c r="N12" t="n">
+        <v>30442.11945677995</v>
+      </c>
+      <c r="O12" t="n">
+        <v>2.69</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.01709590679277717</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>801.7464</v>
+      </c>
+      <c r="R12" t="n">
+        <v>1.0493</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0.0481</v>
+      </c>
+      <c r="T12" t="n">
+        <v>4.5827</v>
+      </c>
+      <c r="U12" t="n">
+        <v>18.3006</v>
+      </c>
+      <c r="V12" t="n">
+        <v>7.4675</v>
+      </c>
+      <c r="W12" t="n">
+        <v>3.4064</v>
+      </c>
+      <c r="X12" t="n">
+        <v>0.3994222222222221</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>22.53893635749351</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>0.1362610777145619</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>41.622</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>42.951</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>1.0619</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>75%</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>7</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2022</v>
+      </c>
+      <c r="G13" t="n">
+        <v>40.71018981933594</v>
+      </c>
+      <c r="H13" t="n">
+        <v>78.59722900390625</v>
+      </c>
+      <c r="I13" t="n">
+        <v>25.66505432128906</v>
+      </c>
+      <c r="J13" t="n">
+        <v>21.59468460083008</v>
+      </c>
+      <c r="K13" t="n">
+        <v>538.0977263972998</v>
+      </c>
+      <c r="L13" t="n">
+        <v>1615.124182631494</v>
+      </c>
+      <c r="M13" t="n">
+        <v>1909.229606310153</v>
+      </c>
+      <c r="N13" t="n">
+        <v>67469.80603896419</v>
+      </c>
+      <c r="O13" t="n">
+        <v>7.065</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.1927567260325882</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>2634.39155</v>
+      </c>
+      <c r="R13" t="n">
+        <v>3.5208</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0.170775</v>
+      </c>
+      <c r="T13" t="n">
+        <v>50.908</v>
+      </c>
+      <c r="U13" t="n">
+        <v>33.62885</v>
+      </c>
+      <c r="V13" t="n">
+        <v>16.6238</v>
+      </c>
+      <c r="W13" t="n">
+        <v>8.552</v>
+      </c>
+      <c r="X13" t="n">
+        <v>4.425665625000001</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>31.28962366247985</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>0.4921802754905359</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>62.008</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>63.656</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>1.61135</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
           <t>max</t>
         </is>
       </c>
-      <c r="D12" t="n">
+      <c r="D14" t="n">
         <v>12</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E14" t="n">
         <v>2023</v>
       </c>
-      <c r="G12" t="n">
+      <c r="G14" t="n">
         <v>71.38114929199219</v>
       </c>
-      <c r="H12" t="n">
+      <c r="H14" t="n">
         <v>97.50150299072266</v>
       </c>
-      <c r="I12" t="n">
+      <c r="I14" t="n">
         <v>68.07738494873047</v>
       </c>
-      <c r="J12" t="n">
+      <c r="J14" t="n">
         <v>75.83811187744141</v>
       </c>
-      <c r="K12" t="n">
+      <c r="K14" t="n">
         <v>4264.174377568997</v>
       </c>
-      <c r="L12" t="n">
+      <c r="L14" t="n">
         <v>6417.569987869821</v>
       </c>
-      <c r="M12" t="n">
+      <c r="M14" t="n">
         <v>5676.311159455392</v>
       </c>
-      <c r="N12" t="n">
+      <c r="N14" t="n">
         <v>363706.1196429119</v>
       </c>
-      <c r="O12" t="n">
+      <c r="O14" t="n">
         <v>312.05</v>
       </c>
-      <c r="P12" t="n">
+      <c r="P14" t="n">
+        <v>18.89583333333333</v>
+      </c>
+      <c r="Q14" t="n">
         <v>101282.5255</v>
       </c>
-      <c r="Q12" t="n">
+      <c r="R14" t="n">
         <v>87.1399</v>
       </c>
-      <c r="R12" t="n">
+      <c r="S14" t="n">
         <v>22.27</v>
       </c>
-      <c r="S12" t="n">
+      <c r="T14" t="n">
         <v>28892</v>
       </c>
-      <c r="T12" t="n">
+      <c r="U14" t="n">
         <v>4367.8691</v>
       </c>
-      <c r="U12" t="n">
+      <c r="V14" t="n">
         <v>5208.6957</v>
       </c>
-      <c r="V12" t="n">
+      <c r="W14" t="n">
         <v>236.0122</v>
       </c>
-      <c r="W12" t="n">
+      <c r="X14" t="n">
+        <v>10.871953125</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>41.9745064904734</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>6.221893112792712</v>
+      </c>
+      <c r="AA14" t="n">
         <v>376.901</v>
       </c>
-      <c r="X12" t="n">
+      <c r="AB14" t="n">
         <v>323.994</v>
       </c>
-      <c r="Y12" t="n">
+      <c r="AC14" t="n">
         <v>25.11</v>
       </c>
     </row>
@@ -1248,27 +1385,27 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>year</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>sec_no</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>tkr</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="3" t="n">
         <v>2017</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C2" t="n">
@@ -1276,8 +1413,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="n"/>
-      <c r="B3" s="2" t="n">
+      <c r="A3" s="4" t="n"/>
+      <c r="B3" s="3" t="n">
         <v>2</v>
       </c>
       <c r="C3" t="n">
@@ -1285,8 +1422,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="n"/>
-      <c r="B4" s="2" t="n">
+      <c r="A4" s="4" t="n"/>
+      <c r="B4" s="3" t="n">
         <v>3</v>
       </c>
       <c r="C4" t="n">
@@ -1294,8 +1431,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="n"/>
-      <c r="B5" s="2" t="n">
+      <c r="A5" s="4" t="n"/>
+      <c r="B5" s="3" t="n">
         <v>4</v>
       </c>
       <c r="C5" t="n">
@@ -1303,8 +1440,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="n"/>
-      <c r="B6" s="2" t="n">
+      <c r="A6" s="4" t="n"/>
+      <c r="B6" s="3" t="n">
         <v>5</v>
       </c>
       <c r="C6" t="n">
@@ -1312,8 +1449,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="n"/>
-      <c r="B7" s="2" t="n">
+      <c r="A7" s="4" t="n"/>
+      <c r="B7" s="3" t="n">
         <v>6</v>
       </c>
       <c r="C7" t="n">
@@ -1321,8 +1458,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="n"/>
-      <c r="B8" s="2" t="n">
+      <c r="A8" s="4" t="n"/>
+      <c r="B8" s="3" t="n">
         <v>7</v>
       </c>
       <c r="C8" t="n">
@@ -1330,8 +1467,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="n"/>
-      <c r="B9" s="2" t="n">
+      <c r="A9" s="4" t="n"/>
+      <c r="B9" s="3" t="n">
         <v>8</v>
       </c>
       <c r="C9" t="n">
@@ -1339,8 +1476,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="n"/>
-      <c r="B10" s="2" t="n">
+      <c r="A10" s="4" t="n"/>
+      <c r="B10" s="3" t="n">
         <v>9</v>
       </c>
       <c r="C10" t="n">
@@ -1348,8 +1485,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="n"/>
-      <c r="B11" s="2" t="n">
+      <c r="A11" s="4" t="n"/>
+      <c r="B11" s="3" t="n">
         <v>10</v>
       </c>
       <c r="C11" t="n">
@@ -1357,8 +1494,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="n"/>
-      <c r="B12" s="2" t="n">
+      <c r="A12" s="4" t="n"/>
+      <c r="B12" s="3" t="n">
         <v>11</v>
       </c>
       <c r="C12" t="n">
@@ -1366,8 +1503,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="4" t="n"/>
-      <c r="B13" s="2" t="n">
+      <c r="A13" s="5" t="n"/>
+      <c r="B13" s="3" t="n">
         <v>12</v>
       </c>
       <c r="C13" t="n">
@@ -1375,10 +1512,10 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="n">
+      <c r="A14" s="3" t="n">
         <v>2018</v>
       </c>
-      <c r="B14" s="2" t="n">
+      <c r="B14" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C14" t="n">
@@ -1386,8 +1523,8 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="n"/>
-      <c r="B15" s="2" t="n">
+      <c r="A15" s="4" t="n"/>
+      <c r="B15" s="3" t="n">
         <v>2</v>
       </c>
       <c r="C15" t="n">
@@ -1395,8 +1532,8 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="3" t="n"/>
-      <c r="B16" s="2" t="n">
+      <c r="A16" s="4" t="n"/>
+      <c r="B16" s="3" t="n">
         <v>3</v>
       </c>
       <c r="C16" t="n">
@@ -1404,8 +1541,8 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="3" t="n"/>
-      <c r="B17" s="2" t="n">
+      <c r="A17" s="4" t="n"/>
+      <c r="B17" s="3" t="n">
         <v>4</v>
       </c>
       <c r="C17" t="n">
@@ -1413,8 +1550,8 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="n"/>
-      <c r="B18" s="2" t="n">
+      <c r="A18" s="4" t="n"/>
+      <c r="B18" s="3" t="n">
         <v>5</v>
       </c>
       <c r="C18" t="n">
@@ -1422,8 +1559,8 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="3" t="n"/>
-      <c r="B19" s="2" t="n">
+      <c r="A19" s="4" t="n"/>
+      <c r="B19" s="3" t="n">
         <v>6</v>
       </c>
       <c r="C19" t="n">
@@ -1431,8 +1568,8 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="3" t="n"/>
-      <c r="B20" s="2" t="n">
+      <c r="A20" s="4" t="n"/>
+      <c r="B20" s="3" t="n">
         <v>7</v>
       </c>
       <c r="C20" t="n">
@@ -1440,8 +1577,8 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="3" t="n"/>
-      <c r="B21" s="2" t="n">
+      <c r="A21" s="4" t="n"/>
+      <c r="B21" s="3" t="n">
         <v>8</v>
       </c>
       <c r="C21" t="n">
@@ -1449,8 +1586,8 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="3" t="n"/>
-      <c r="B22" s="2" t="n">
+      <c r="A22" s="4" t="n"/>
+      <c r="B22" s="3" t="n">
         <v>9</v>
       </c>
       <c r="C22" t="n">
@@ -1458,8 +1595,8 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="3" t="n"/>
-      <c r="B23" s="2" t="n">
+      <c r="A23" s="4" t="n"/>
+      <c r="B23" s="3" t="n">
         <v>10</v>
       </c>
       <c r="C23" t="n">
@@ -1467,8 +1604,8 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="3" t="n"/>
-      <c r="B24" s="2" t="n">
+      <c r="A24" s="4" t="n"/>
+      <c r="B24" s="3" t="n">
         <v>11</v>
       </c>
       <c r="C24" t="n">
@@ -1476,8 +1613,8 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="4" t="n"/>
-      <c r="B25" s="2" t="n">
+      <c r="A25" s="5" t="n"/>
+      <c r="B25" s="3" t="n">
         <v>12</v>
       </c>
       <c r="C25" t="n">
@@ -1485,10 +1622,10 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="2" t="n">
+      <c r="A26" s="3" t="n">
         <v>2019</v>
       </c>
-      <c r="B26" s="2" t="n">
+      <c r="B26" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C26" t="n">
@@ -1496,8 +1633,8 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="3" t="n"/>
-      <c r="B27" s="2" t="n">
+      <c r="A27" s="4" t="n"/>
+      <c r="B27" s="3" t="n">
         <v>2</v>
       </c>
       <c r="C27" t="n">
@@ -1505,8 +1642,8 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="3" t="n"/>
-      <c r="B28" s="2" t="n">
+      <c r="A28" s="4" t="n"/>
+      <c r="B28" s="3" t="n">
         <v>3</v>
       </c>
       <c r="C28" t="n">
@@ -1514,8 +1651,8 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="3" t="n"/>
-      <c r="B29" s="2" t="n">
+      <c r="A29" s="4" t="n"/>
+      <c r="B29" s="3" t="n">
         <v>4</v>
       </c>
       <c r="C29" t="n">
@@ -1523,8 +1660,8 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="3" t="n"/>
-      <c r="B30" s="2" t="n">
+      <c r="A30" s="4" t="n"/>
+      <c r="B30" s="3" t="n">
         <v>5</v>
       </c>
       <c r="C30" t="n">
@@ -1532,8 +1669,8 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="3" t="n"/>
-      <c r="B31" s="2" t="n">
+      <c r="A31" s="4" t="n"/>
+      <c r="B31" s="3" t="n">
         <v>6</v>
       </c>
       <c r="C31" t="n">
@@ -1541,8 +1678,8 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="3" t="n"/>
-      <c r="B32" s="2" t="n">
+      <c r="A32" s="4" t="n"/>
+      <c r="B32" s="3" t="n">
         <v>7</v>
       </c>
       <c r="C32" t="n">
@@ -1550,8 +1687,8 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="3" t="n"/>
-      <c r="B33" s="2" t="n">
+      <c r="A33" s="4" t="n"/>
+      <c r="B33" s="3" t="n">
         <v>8</v>
       </c>
       <c r="C33" t="n">
@@ -1559,8 +1696,8 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="3" t="n"/>
-      <c r="B34" s="2" t="n">
+      <c r="A34" s="4" t="n"/>
+      <c r="B34" s="3" t="n">
         <v>9</v>
       </c>
       <c r="C34" t="n">
@@ -1568,8 +1705,8 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="3" t="n"/>
-      <c r="B35" s="2" t="n">
+      <c r="A35" s="4" t="n"/>
+      <c r="B35" s="3" t="n">
         <v>10</v>
       </c>
       <c r="C35" t="n">
@@ -1577,8 +1714,8 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="3" t="n"/>
-      <c r="B36" s="2" t="n">
+      <c r="A36" s="4" t="n"/>
+      <c r="B36" s="3" t="n">
         <v>11</v>
       </c>
       <c r="C36" t="n">
@@ -1586,8 +1723,8 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="4" t="n"/>
-      <c r="B37" s="2" t="n">
+      <c r="A37" s="5" t="n"/>
+      <c r="B37" s="3" t="n">
         <v>12</v>
       </c>
       <c r="C37" t="n">
@@ -1595,10 +1732,10 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="2" t="n">
+      <c r="A38" s="3" t="n">
         <v>2020</v>
       </c>
-      <c r="B38" s="2" t="n">
+      <c r="B38" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C38" t="n">
@@ -1606,8 +1743,8 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="3" t="n"/>
-      <c r="B39" s="2" t="n">
+      <c r="A39" s="4" t="n"/>
+      <c r="B39" s="3" t="n">
         <v>2</v>
       </c>
       <c r="C39" t="n">
@@ -1615,8 +1752,8 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="3" t="n"/>
-      <c r="B40" s="2" t="n">
+      <c r="A40" s="4" t="n"/>
+      <c r="B40" s="3" t="n">
         <v>3</v>
       </c>
       <c r="C40" t="n">
@@ -1624,8 +1761,8 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="3" t="n"/>
-      <c r="B41" s="2" t="n">
+      <c r="A41" s="4" t="n"/>
+      <c r="B41" s="3" t="n">
         <v>4</v>
       </c>
       <c r="C41" t="n">
@@ -1633,8 +1770,8 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="3" t="n"/>
-      <c r="B42" s="2" t="n">
+      <c r="A42" s="4" t="n"/>
+      <c r="B42" s="3" t="n">
         <v>5</v>
       </c>
       <c r="C42" t="n">
@@ -1642,8 +1779,8 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="3" t="n"/>
-      <c r="B43" s="2" t="n">
+      <c r="A43" s="4" t="n"/>
+      <c r="B43" s="3" t="n">
         <v>6</v>
       </c>
       <c r="C43" t="n">
@@ -1651,8 +1788,8 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="3" t="n"/>
-      <c r="B44" s="2" t="n">
+      <c r="A44" s="4" t="n"/>
+      <c r="B44" s="3" t="n">
         <v>7</v>
       </c>
       <c r="C44" t="n">
@@ -1660,8 +1797,8 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="3" t="n"/>
-      <c r="B45" s="2" t="n">
+      <c r="A45" s="4" t="n"/>
+      <c r="B45" s="3" t="n">
         <v>8</v>
       </c>
       <c r="C45" t="n">
@@ -1669,8 +1806,8 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="3" t="n"/>
-      <c r="B46" s="2" t="n">
+      <c r="A46" s="4" t="n"/>
+      <c r="B46" s="3" t="n">
         <v>9</v>
       </c>
       <c r="C46" t="n">
@@ -1678,8 +1815,8 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="3" t="n"/>
-      <c r="B47" s="2" t="n">
+      <c r="A47" s="4" t="n"/>
+      <c r="B47" s="3" t="n">
         <v>10</v>
       </c>
       <c r="C47" t="n">
@@ -1687,8 +1824,8 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="3" t="n"/>
-      <c r="B48" s="2" t="n">
+      <c r="A48" s="4" t="n"/>
+      <c r="B48" s="3" t="n">
         <v>11</v>
       </c>
       <c r="C48" t="n">
@@ -1696,8 +1833,8 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="4" t="n"/>
-      <c r="B49" s="2" t="n">
+      <c r="A49" s="5" t="n"/>
+      <c r="B49" s="3" t="n">
         <v>12</v>
       </c>
       <c r="C49" t="n">
@@ -1705,10 +1842,10 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="2" t="n">
+      <c r="A50" s="3" t="n">
         <v>2021</v>
       </c>
-      <c r="B50" s="2" t="n">
+      <c r="B50" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C50" t="n">
@@ -1716,8 +1853,8 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="3" t="n"/>
-      <c r="B51" s="2" t="n">
+      <c r="A51" s="4" t="n"/>
+      <c r="B51" s="3" t="n">
         <v>2</v>
       </c>
       <c r="C51" t="n">
@@ -1725,8 +1862,8 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="3" t="n"/>
-      <c r="B52" s="2" t="n">
+      <c r="A52" s="4" t="n"/>
+      <c r="B52" s="3" t="n">
         <v>3</v>
       </c>
       <c r="C52" t="n">
@@ -1734,8 +1871,8 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="3" t="n"/>
-      <c r="B53" s="2" t="n">
+      <c r="A53" s="4" t="n"/>
+      <c r="B53" s="3" t="n">
         <v>4</v>
       </c>
       <c r="C53" t="n">
@@ -1743,8 +1880,8 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="3" t="n"/>
-      <c r="B54" s="2" t="n">
+      <c r="A54" s="4" t="n"/>
+      <c r="B54" s="3" t="n">
         <v>5</v>
       </c>
       <c r="C54" t="n">
@@ -1752,8 +1889,8 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="3" t="n"/>
-      <c r="B55" s="2" t="n">
+      <c r="A55" s="4" t="n"/>
+      <c r="B55" s="3" t="n">
         <v>6</v>
       </c>
       <c r="C55" t="n">
@@ -1761,8 +1898,8 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="3" t="n"/>
-      <c r="B56" s="2" t="n">
+      <c r="A56" s="4" t="n"/>
+      <c r="B56" s="3" t="n">
         <v>7</v>
       </c>
       <c r="C56" t="n">
@@ -1770,8 +1907,8 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="3" t="n"/>
-      <c r="B57" s="2" t="n">
+      <c r="A57" s="4" t="n"/>
+      <c r="B57" s="3" t="n">
         <v>8</v>
       </c>
       <c r="C57" t="n">
@@ -1779,8 +1916,8 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="3" t="n"/>
-      <c r="B58" s="2" t="n">
+      <c r="A58" s="4" t="n"/>
+      <c r="B58" s="3" t="n">
         <v>9</v>
       </c>
       <c r="C58" t="n">
@@ -1788,8 +1925,8 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="3" t="n"/>
-      <c r="B59" s="2" t="n">
+      <c r="A59" s="4" t="n"/>
+      <c r="B59" s="3" t="n">
         <v>10</v>
       </c>
       <c r="C59" t="n">
@@ -1797,8 +1934,8 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="3" t="n"/>
-      <c r="B60" s="2" t="n">
+      <c r="A60" s="4" t="n"/>
+      <c r="B60" s="3" t="n">
         <v>11</v>
       </c>
       <c r="C60" t="n">
@@ -1806,8 +1943,8 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="4" t="n"/>
-      <c r="B61" s="2" t="n">
+      <c r="A61" s="5" t="n"/>
+      <c r="B61" s="3" t="n">
         <v>12</v>
       </c>
       <c r="C61" t="n">
@@ -1815,10 +1952,10 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="2" t="n">
+      <c r="A62" s="3" t="n">
         <v>2022</v>
       </c>
-      <c r="B62" s="2" t="n">
+      <c r="B62" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C62" t="n">
@@ -1826,8 +1963,8 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="3" t="n"/>
-      <c r="B63" s="2" t="n">
+      <c r="A63" s="4" t="n"/>
+      <c r="B63" s="3" t="n">
         <v>2</v>
       </c>
       <c r="C63" t="n">
@@ -1835,8 +1972,8 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="3" t="n"/>
-      <c r="B64" s="2" t="n">
+      <c r="A64" s="4" t="n"/>
+      <c r="B64" s="3" t="n">
         <v>3</v>
       </c>
       <c r="C64" t="n">
@@ -1844,8 +1981,8 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="3" t="n"/>
-      <c r="B65" s="2" t="n">
+      <c r="A65" s="4" t="n"/>
+      <c r="B65" s="3" t="n">
         <v>4</v>
       </c>
       <c r="C65" t="n">
@@ -1853,8 +1990,8 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="3" t="n"/>
-      <c r="B66" s="2" t="n">
+      <c r="A66" s="4" t="n"/>
+      <c r="B66" s="3" t="n">
         <v>5</v>
       </c>
       <c r="C66" t="n">
@@ -1862,8 +1999,8 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="3" t="n"/>
-      <c r="B67" s="2" t="n">
+      <c r="A67" s="4" t="n"/>
+      <c r="B67" s="3" t="n">
         <v>6</v>
       </c>
       <c r="C67" t="n">
@@ -1871,8 +2008,8 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="3" t="n"/>
-      <c r="B68" s="2" t="n">
+      <c r="A68" s="4" t="n"/>
+      <c r="B68" s="3" t="n">
         <v>7</v>
       </c>
       <c r="C68" t="n">
@@ -1880,8 +2017,8 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="3" t="n"/>
-      <c r="B69" s="2" t="n">
+      <c r="A69" s="4" t="n"/>
+      <c r="B69" s="3" t="n">
         <v>8</v>
       </c>
       <c r="C69" t="n">
@@ -1889,8 +2026,8 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="3" t="n"/>
-      <c r="B70" s="2" t="n">
+      <c r="A70" s="4" t="n"/>
+      <c r="B70" s="3" t="n">
         <v>9</v>
       </c>
       <c r="C70" t="n">
@@ -1898,8 +2035,8 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="3" t="n"/>
-      <c r="B71" s="2" t="n">
+      <c r="A71" s="4" t="n"/>
+      <c r="B71" s="3" t="n">
         <v>10</v>
       </c>
       <c r="C71" t="n">
@@ -1907,8 +2044,8 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="3" t="n"/>
-      <c r="B72" s="2" t="n">
+      <c r="A72" s="4" t="n"/>
+      <c r="B72" s="3" t="n">
         <v>11</v>
       </c>
       <c r="C72" t="n">
@@ -1916,8 +2053,8 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="4" t="n"/>
-      <c r="B73" s="2" t="n">
+      <c r="A73" s="5" t="n"/>
+      <c r="B73" s="3" t="n">
         <v>12</v>
       </c>
       <c r="C73" t="n">
@@ -1925,10 +2062,10 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="2" t="n">
+      <c r="A74" s="3" t="n">
         <v>2023</v>
       </c>
-      <c r="B74" s="2" t="n">
+      <c r="B74" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C74" t="n">
@@ -1936,8 +2073,8 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="3" t="n"/>
-      <c r="B75" s="2" t="n">
+      <c r="A75" s="4" t="n"/>
+      <c r="B75" s="3" t="n">
         <v>2</v>
       </c>
       <c r="C75" t="n">
@@ -1945,8 +2082,8 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="3" t="n"/>
-      <c r="B76" s="2" t="n">
+      <c r="A76" s="4" t="n"/>
+      <c r="B76" s="3" t="n">
         <v>3</v>
       </c>
       <c r="C76" t="n">
@@ -1954,8 +2091,8 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="3" t="n"/>
-      <c r="B77" s="2" t="n">
+      <c r="A77" s="4" t="n"/>
+      <c r="B77" s="3" t="n">
         <v>4</v>
       </c>
       <c r="C77" t="n">
@@ -1963,8 +2100,8 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="3" t="n"/>
-      <c r="B78" s="2" t="n">
+      <c r="A78" s="4" t="n"/>
+      <c r="B78" s="3" t="n">
         <v>5</v>
       </c>
       <c r="C78" t="n">
@@ -1972,8 +2109,8 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="3" t="n"/>
-      <c r="B79" s="2" t="n">
+      <c r="A79" s="4" t="n"/>
+      <c r="B79" s="3" t="n">
         <v>6</v>
       </c>
       <c r="C79" t="n">
@@ -1981,8 +2118,8 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="3" t="n"/>
-      <c r="B80" s="2" t="n">
+      <c r="A80" s="4" t="n"/>
+      <c r="B80" s="3" t="n">
         <v>7</v>
       </c>
       <c r="C80" t="n">
@@ -1990,8 +2127,8 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="3" t="n"/>
-      <c r="B81" s="2" t="n">
+      <c r="A81" s="4" t="n"/>
+      <c r="B81" s="3" t="n">
         <v>8</v>
       </c>
       <c r="C81" t="n">
@@ -1999,8 +2136,8 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="3" t="n"/>
-      <c r="B82" s="2" t="n">
+      <c r="A82" s="4" t="n"/>
+      <c r="B82" s="3" t="n">
         <v>9</v>
       </c>
       <c r="C82" t="n">
@@ -2008,8 +2145,8 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="3" t="n"/>
-      <c r="B83" s="2" t="n">
+      <c r="A83" s="4" t="n"/>
+      <c r="B83" s="3" t="n">
         <v>10</v>
       </c>
       <c r="C83" t="n">
@@ -2017,8 +2154,8 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="3" t="n"/>
-      <c r="B84" s="2" t="n">
+      <c r="A84" s="4" t="n"/>
+      <c r="B84" s="3" t="n">
         <v>11</v>
       </c>
       <c r="C84" t="n">
@@ -2026,8 +2163,8 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="4" t="n"/>
-      <c r="B85" s="2" t="n">
+      <c r="A85" s="5" t="n"/>
+      <c r="B85" s="3" t="n">
         <v>12</v>
       </c>
       <c r="C85" t="n">
@@ -2054,7 +2191,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2063,12 +2200,12 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>variable</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>kurtosis</t>
         </is>
@@ -2081,7 +2218,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.8439973623210526</v>
+        <v>-0.8433297793275281</v>
       </c>
     </row>
     <row r="3">
@@ -2091,7 +2228,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-1.338866040737074</v>
+        <v>-1.250106653882256</v>
       </c>
     </row>
     <row r="4">
@@ -2101,7 +2238,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.5804825796085802</v>
+        <v>0.4984350574899099</v>
       </c>
     </row>
     <row r="5">
@@ -2111,7 +2248,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2.286529271087936</v>
+        <v>2.486789225007624</v>
       </c>
     </row>
     <row r="6">
@@ -2121,7 +2258,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.451304610453001</v>
+        <v>1.372140166008562</v>
       </c>
     </row>
     <row r="7">
@@ -2131,7 +2268,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.011395896788574</v>
+        <v>0.868593777724088</v>
       </c>
     </row>
     <row r="8">
@@ -2141,7 +2278,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>6.173728941689481</v>
+        <v>5.831489896738807</v>
       </c>
     </row>
     <row r="9">
@@ -2151,7 +2288,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1.699884465364931</v>
+        <v>1.55229652780931</v>
       </c>
     </row>
     <row r="10">
@@ -2161,7 +2298,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1.925157623025872</v>
+        <v>1.806517378766842</v>
       </c>
     </row>
     <row r="11">
@@ -2171,7 +2308,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>5.20856954441853</v>
+        <v>4.942924347619279</v>
       </c>
     </row>
     <row r="12">
@@ -2181,117 +2318,157 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>62.39343682450749</v>
+        <v>62.35545019128232</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>historical_market_cap</t>
+          <t>ret</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>38.5796037820777</v>
+        <v>190.0181459437518</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>trail_12m_sales_per_sh</t>
+          <t>historical_market_cap</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>25.25846748607098</v>
+        <v>37.84559988809755</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>is_eps</t>
+          <t>trail_12m_sales_per_sh</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>252.5539200037411</v>
+        <v>25.7082139692149</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>fcf</t>
+          <t>is_eps</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>266.5751788276784</v>
+        <v>263.1165927204931</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>pe</t>
+          <t>fcf</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>133.2680418278964</v>
+        <v>260.4654653211155</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>return_com_eqy</t>
+          <t>pe</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1010.161312293044</v>
+        <v>119.9591360380189</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>roa</t>
+          <t>return_com_eqy</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>22.12475707567043</v>
+        <v>909.6147485647926</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>VOLATILITY_180D</t>
+          <t>roa</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>15.700676508373</v>
+        <v>22.22640631216099</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>volatility_360d</t>
+          <t>roa_sec_mean</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>11.22111393360461</v>
+        <v>-1.057225331911546</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>beta</t>
+          <t>roa_sec_sd</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>74.03672747771991</v>
+        <v>-1.303093626177318</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>roa_z</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>5.918586843393905</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>vol_180d</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>16.87112843931878</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>vol_360d</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>12.1497697511229</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>beta</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>85.87137069051082</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
           <t>kurtosis_mean</t>
         </is>
       </c>
-      <c r="B23" t="n">
-        <v>91.90606788427442</v>
+      <c r="B27" t="n">
+        <v>81.08104182636559</v>
       </c>
     </row>
   </sheetData>

</xml_diff>